<commit_message>
adding support to Excel reporter
</commit_message>
<xml_diff>
--- a/t/test_out.mine.xlsx
+++ b/t/test_out.mine.xlsx
@@ -8,13 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
+    <sheet name="values" sheetId="2" r:id="rId2"/>
+    <sheet name="units" sheetId="3" r:id="rId3"/>
+    <sheet name="uris" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -65,6 +68,78 @@
   </si>
   <si>
     <t>S011JHDN1</t>
+  </si>
+  <si>
+    <t>SAMPLE</t>
+  </si>
+  <si>
+    <t>Pippo</t>
+  </si>
+  <si>
+    <t>Primary Tissue</t>
+  </si>
+  <si>
+    <t>Venous blood</t>
+  </si>
+  <si>
+    <t>median cubital vein</t>
+  </si>
+  <si>
+    <t>S011JH</t>
+  </si>
+  <si>
+    <t>50-55</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UBERON_0013756</t>
+  </si>
+  <si>
+    <t>UBERON_0013756</t>
+  </si>
+  <si>
+    <t>ERC000026</t>
+  </si>
+  <si>
+    <t>S00DQ0N2</t>
+  </si>
+  <si>
+    <t>NIHR Cambridge BioResource</t>
+  </si>
+  <si>
+    <t>S00DQ0</t>
+  </si>
+  <si>
+    <t>50- 55</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>total RNA</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>uri</t>
   </si>
 </sst>
 </file>
@@ -88,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,15 +172,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -123,10 +219,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,65 +520,445 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>